<commit_message>
Set 1 de instancias
</commit_message>
<xml_diff>
--- a/Codes/Tesis/LocalSearch/ExperimentosProbVerif1.xlsx
+++ b/Codes/Tesis/LocalSearch/ExperimentosProbVerif1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Documents\EstudiosProfesionales\FIME\Doctorado\TesisDoctoral\Codes\Tesis\LocalSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52704C78-9111-4083-A49B-54AFE53B56F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0371C8-17DF-4EA4-BB2E-C9DB6A193775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DB165B49-1477-4F86-B9E4-42190450FB18}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Instance_168_16_10_6_6_Exp13</t>
+  </si>
+  <si>
+    <t>probVerif</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7341436D-B043-45EF-9D55-56F4C62775C5}">
-  <dimension ref="B2:H15"/>
+  <dimension ref="B2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +485,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -505,7 +508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -528,7 +531,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -551,7 +554,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -574,7 +577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -597,7 +600,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -620,7 +623,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -643,7 +646,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -666,7 +669,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -688,8 +691,11 @@
       <c r="H10">
         <v>3.7600000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -712,7 +718,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -735,7 +741,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -758,7 +764,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -781,7 +787,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>

</xml_diff>